<commit_message>
changed attribs to mref where applicable
</commit_message>
<xml_diff>
--- a/dist/rd3.2.0-beta-0.9.5.xlsx
+++ b/dist/rd3.2.0-beta-0.9.5.xlsx
@@ -1762,334 +1762,334 @@
     <t>rangeMax</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42883</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C61512</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_000087</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ExO_0000127</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C15607</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25461</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/SCDO_0002829</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C172217</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C63536</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C171105</t>
   </si>
   <si>
-    <t>http://semanticscience.org/resource/SIO_000087</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C47824</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C172217</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25461</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C15607</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42883</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C61512</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/SCDO_0002829</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C63536</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C25412</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/ExO_0000127</t>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C176375</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C49100</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C183337</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171103</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171337</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171191</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C69208</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_000670</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/FIX_0000704</t>
+  </si>
+  <si>
+    <t>http://www.ebi.ac.uk/efo/EFO_0005518</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C127771</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIABIS_0000006</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70713</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C53190</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C16493</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171252</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C93629</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/SNOMEDCT/423493009</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C43361</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25393</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25173</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001891</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25365</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C93495</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/ICO_0000178</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GENEPIO_0001921</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0500027</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C16977</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIT_0004546</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C164483</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C93400</t>
+  </si>
+  <si>
+    <t>https://w3id.org/reproduceme#doi</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C94324</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C171276</t>
+  </si>
+  <si>
+    <t>http://edamontology.org/data_3273</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C40976</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIABIS_0000100</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C153145</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C64917</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_001330</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C40975</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C142702</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C135383</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C142495</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GSSO_001755</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DUO_0000001</t>
   </si>
   <si>
     <t>http://www.orpha.net/ORDO/Orphanet_C023</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/OMIABIS_0000100</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171337</t>
+    <t>http://semanticscience.org/resource/SIO_001083</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OMIABIS_0000037</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42628</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C47922</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C115505</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C19924</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C90353</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C67073</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42775</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25737</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C103264</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/OMIABIS_0000035</t>
   </si>
   <si>
-    <t>https://w3id.org/reproduceme#doi</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C16493</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/ICO_0000178</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C90353</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
+    <t>http://purl.obolibrary.org/obo/GO_0001894</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C40974</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C93495</t>
+    <t>http://purl.obolibrary.org/obo/NCIT_C16735</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/RO_0000056</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C166209</t>
+  </si>
+  <si>
+    <t>http://semanticscience.org/resource/SIO_000669</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C166237</t>
+  </si>
+  <si>
+    <t>https://w3id.org/reproduceme#wasUpdatedBy</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C176373</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42614</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C89336</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C142704</t>
+  </si>
+  <si>
+    <t>http://purl.bioontology.org/ontology/HL7/C0442737</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C83164</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/GENEPIO_0001094</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C16735</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C19924</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25173</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C16977</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C183337</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OMIT_0004546</t>
-  </si>
-  <si>
-    <t>http://www.ebi.ac.uk/efo/EFO_0005518</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42628</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GENEPIO_0001921</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C69208</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C153145</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171276</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GSSO_001755</t>
-  </si>
-  <si>
-    <t>http://purl.bioontology.org/ontology/SNOMEDCT/423493009</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C166237</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171191</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OMIABIS_0000037</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OMIABIS_0000006</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C103264</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/FIX_0000704</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C93400</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C64917</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/SIO_001330</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C43361</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C89336</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C142495</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C135383</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C94324</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/RO_0000056</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/SIO_000669</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C176373</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42775</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/SIO_000670</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C166209</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C127771</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C164483</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C67073</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBI_0001891</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/GO_0001894</t>
-  </si>
-  <si>
-    <t>http://semanticscience.org/resource/SIO_001083</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171252</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C47922</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C70713</t>
-  </si>
-  <si>
-    <t>http://purl.bioontology.org/ontology/HL7/C0442737</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C40976</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C142702</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/OBI_0500027</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C115505</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C93629</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42614</t>
-  </si>
-  <si>
-    <t>https://w3id.org/reproduceme#wasUpdatedBy</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25737</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25393</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C40975</t>
-  </si>
-  <si>
-    <t>http://edamontology.org/data_3273</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C171103</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C176375</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C83164</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25365</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/DUO_0000001</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C49100</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C53190</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C142704</t>
-  </si>
-  <si>
     <t>NCIT</t>
   </si>
   <si>
     <t>SIO</t>
   </si>
   <si>
+    <t>ExO</t>
+  </si>
+  <si>
     <t>SCDO</t>
   </si>
   <si>
-    <t>ExO</t>
+    <t>FIX</t>
+  </si>
+  <si>
+    <t>EFO</t>
+  </si>
+  <si>
+    <t>OMIABIS</t>
+  </si>
+  <si>
+    <t>SNOMEDCT</t>
+  </si>
+  <si>
+    <t>OBI</t>
+  </si>
+  <si>
+    <t>ICO</t>
+  </si>
+  <si>
+    <t>GENEPIO</t>
+  </si>
+  <si>
+    <t>OMIT</t>
+  </si>
+  <si>
+    <t>reproduceme</t>
+  </si>
+  <si>
+    <t>EDAM</t>
+  </si>
+  <si>
+    <t>GSSO</t>
+  </si>
+  <si>
+    <t>DUO</t>
   </si>
   <si>
     <t>Orphanet</t>
   </si>
   <si>
-    <t>OMIABIS</t>
-  </si>
-  <si>
-    <t>reproduceme</t>
-  </si>
-  <si>
-    <t>ICO</t>
-  </si>
-  <si>
-    <t>GENEPIO</t>
-  </si>
-  <si>
-    <t>OMIT</t>
-  </si>
-  <si>
-    <t>EFO</t>
-  </si>
-  <si>
-    <t>GSSO</t>
-  </si>
-  <si>
-    <t>SNOMEDCT</t>
-  </si>
-  <si>
-    <t>FIX</t>
+    <t>GO</t>
   </si>
   <si>
     <t>RO</t>
   </si>
   <si>
-    <t>OBI</t>
-  </si>
-  <si>
-    <t>GO</t>
-  </si>
-  <si>
     <t>HL7</t>
-  </si>
-  <si>
-    <t>EDAM</t>
-  </si>
-  <si>
-    <t>DUO</t>
   </si>
   <si>
     <t>isAssociatedWith</t>
@@ -3846,7 +3846,7 @@
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="L17" t="b">
         <v>1</v>
@@ -3893,7 +3893,7 @@
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="L18" t="b">
         <v>1</v>
@@ -6781,7 +6781,7 @@
         <v>0</v>
       </c>
       <c r="K85" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="L85" t="b">
         <v>1</v>
@@ -12697,10 +12697,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>581</v>
@@ -12717,16 +12717,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>582</v>
       </c>
       <c r="D3" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E3" t="s">
         <v>691</v>
@@ -12737,16 +12737,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>583</v>
       </c>
       <c r="D4" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="E4" t="s">
         <v>691</v>
@@ -12757,16 +12757,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>584</v>
       </c>
       <c r="D5" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
       <c r="E5" t="s">
         <v>691</v>
@@ -12777,10 +12777,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>585</v>
@@ -12797,10 +12797,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>586</v>
@@ -12817,16 +12817,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>587</v>
       </c>
       <c r="D8" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="E8" t="s">
         <v>691</v>
@@ -12837,10 +12837,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>588</v>
@@ -12857,16 +12857,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>589</v>
       </c>
       <c r="D10" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="E10" t="s">
         <v>691</v>
@@ -12877,10 +12877,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>590</v>
@@ -12897,10 +12897,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>591</v>
@@ -12917,16 +12917,16 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B13" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>592</v>
       </c>
       <c r="D13" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="E13" t="s">
         <v>691</v>
@@ -12937,16 +12937,16 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>460</v>
+        <v>499</v>
       </c>
       <c r="B14" t="s">
-        <v>460</v>
+        <v>499</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>593</v>
       </c>
       <c r="D14" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="E14" t="s">
         <v>691</v>
@@ -12957,16 +12957,16 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="B15" t="s">
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>594</v>
       </c>
       <c r="D15" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="E15" t="s">
         <v>691</v>
@@ -12977,10 +12977,10 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>480</v>
+        <v>497</v>
       </c>
       <c r="B16" t="s">
-        <v>480</v>
+        <v>497</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>595</v>
@@ -12997,16 +12997,16 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>488</v>
+        <v>508</v>
       </c>
       <c r="B17" t="s">
-        <v>488</v>
+        <v>508</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>596</v>
       </c>
       <c r="D17" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="E17" t="s">
         <v>691</v>
@@ -13017,16 +13017,16 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>507</v>
+        <v>519</v>
       </c>
       <c r="B18" t="s">
-        <v>507</v>
+        <v>519</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>597</v>
       </c>
       <c r="D18" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
       <c r="E18" t="s">
         <v>691</v>
@@ -13037,10 +13037,10 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>492</v>
+        <v>480</v>
       </c>
       <c r="B19" t="s">
-        <v>492</v>
+        <v>480</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>598</v>
@@ -13057,16 +13057,16 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>450</v>
+        <v>477</v>
       </c>
       <c r="B20" t="s">
-        <v>450</v>
+        <v>477</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>599</v>
       </c>
       <c r="D20" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="E20" t="s">
         <v>691</v>
@@ -13077,10 +13077,10 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>465</v>
+        <v>517</v>
       </c>
       <c r="B21" t="s">
-        <v>465</v>
+        <v>517</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>600</v>
@@ -13097,16 +13097,16 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B22" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>601</v>
       </c>
       <c r="D22" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="E22" t="s">
         <v>691</v>
@@ -13117,16 +13117,16 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>503</v>
+        <v>476</v>
       </c>
       <c r="B23" t="s">
-        <v>503</v>
+        <v>476</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>602</v>
       </c>
       <c r="D23" t="s">
-        <v>671</v>
+        <v>675</v>
       </c>
       <c r="E23" t="s">
         <v>691</v>
@@ -13137,13 +13137,13 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B24" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="D24" t="s">
         <v>671</v>
@@ -13157,16 +13157,16 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>483</v>
+        <v>469</v>
       </c>
       <c r="B25" t="s">
-        <v>483</v>
+        <v>469</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>603</v>
       </c>
       <c r="D25" t="s">
-        <v>671</v>
+        <v>676</v>
       </c>
       <c r="E25" t="s">
         <v>691</v>
@@ -13177,16 +13177,16 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="B26" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>604</v>
       </c>
       <c r="D26" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
       <c r="E26" t="s">
         <v>691</v>
@@ -13197,16 +13197,16 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>449</v>
+        <v>510</v>
       </c>
       <c r="B27" t="s">
-        <v>449</v>
+        <v>510</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>605</v>
       </c>
       <c r="D27" t="s">
-        <v>671</v>
+        <v>677</v>
       </c>
       <c r="E27" t="s">
         <v>691</v>
@@ -13217,10 +13217,10 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>513</v>
+        <v>468</v>
       </c>
       <c r="B28" t="s">
-        <v>513</v>
+        <v>468</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>606</v>
@@ -13237,10 +13237,10 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>442</v>
+        <v>489</v>
       </c>
       <c r="B29" t="s">
-        <v>442</v>
+        <v>489</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>607</v>
@@ -13257,10 +13257,10 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>446</v>
+        <v>492</v>
       </c>
       <c r="B30" t="s">
-        <v>446</v>
+        <v>492</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>608</v>
@@ -13277,13 +13277,13 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="B31" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>585</v>
+        <v>609</v>
       </c>
       <c r="D31" t="s">
         <v>671</v>
@@ -13297,13 +13297,13 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>508</v>
+        <v>455</v>
       </c>
       <c r="B32" t="s">
-        <v>508</v>
+        <v>455</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="D32" t="s">
         <v>671</v>
@@ -13317,16 +13317,16 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B33" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="D33" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="E33" t="s">
         <v>691</v>
@@ -13337,16 +13337,16 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="B34" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="D34" t="s">
-        <v>681</v>
+        <v>671</v>
       </c>
       <c r="E34" t="s">
         <v>691</v>
@@ -13357,13 +13357,13 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="B35" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="D35" t="s">
         <v>671</v>
@@ -13377,16 +13377,16 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>475</v>
+        <v>442</v>
       </c>
       <c r="B36" t="s">
-        <v>475</v>
+        <v>442</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="D36" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
       <c r="E36" t="s">
         <v>691</v>
@@ -13397,16 +13397,16 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>517</v>
+        <v>474</v>
       </c>
       <c r="B37" t="s">
-        <v>517</v>
+        <v>474</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="D37" t="s">
-        <v>671</v>
+        <v>679</v>
       </c>
       <c r="E37" t="s">
         <v>691</v>
@@ -13417,13 +13417,13 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>520</v>
+        <v>490</v>
       </c>
       <c r="B38" t="s">
-        <v>520</v>
+        <v>490</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D38" t="s">
         <v>671</v>
@@ -13437,13 +13437,13 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="B39" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="D39" t="s">
         <v>671</v>
@@ -13457,16 +13457,16 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>502</v>
+        <v>450</v>
       </c>
       <c r="B40" t="s">
-        <v>502</v>
+        <v>450</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="D40" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="E40" t="s">
         <v>691</v>
@@ -13477,16 +13477,16 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>461</v>
+        <v>120</v>
       </c>
       <c r="B41" t="s">
-        <v>461</v>
+        <v>120</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>618</v>
+        <v>585</v>
       </c>
       <c r="D41" t="s">
-        <v>683</v>
+        <v>671</v>
       </c>
       <c r="E41" t="s">
         <v>691</v>
@@ -13497,16 +13497,16 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>504</v>
+        <v>475</v>
       </c>
       <c r="B42" t="s">
-        <v>504</v>
+        <v>475</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>619</v>
       </c>
       <c r="D42" t="s">
-        <v>671</v>
+        <v>681</v>
       </c>
       <c r="E42" t="s">
         <v>691</v>
@@ -13517,16 +13517,16 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>477</v>
+        <v>512</v>
       </c>
       <c r="B43" t="s">
-        <v>477</v>
+        <v>512</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>620</v>
       </c>
       <c r="D43" t="s">
-        <v>671</v>
+        <v>679</v>
       </c>
       <c r="E43" t="s">
         <v>691</v>
@@ -13537,16 +13537,16 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>511</v>
+        <v>446</v>
       </c>
       <c r="B44" t="s">
-        <v>511</v>
+        <v>446</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>621</v>
       </c>
       <c r="D44" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="E44" t="s">
         <v>691</v>
@@ -13557,16 +13557,16 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>510</v>
+        <v>463</v>
       </c>
       <c r="B45" t="s">
-        <v>510</v>
+        <v>463</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>622</v>
       </c>
       <c r="D45" t="s">
-        <v>676</v>
+        <v>682</v>
       </c>
       <c r="E45" t="s">
         <v>691</v>
@@ -13577,10 +13577,10 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>470</v>
+        <v>453</v>
       </c>
       <c r="B46" t="s">
-        <v>470</v>
+        <v>453</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>623</v>
@@ -13597,16 +13597,16 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="B47" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>624</v>
       </c>
       <c r="D47" t="s">
-        <v>684</v>
+        <v>671</v>
       </c>
       <c r="E47" t="s">
         <v>691</v>
@@ -13623,7 +13623,7 @@
         <v>501</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D48" t="s">
         <v>671</v>
@@ -13643,7 +13643,7 @@
         <v>472</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D49" t="s">
         <v>671</v>
@@ -13657,16 +13657,16 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>115</v>
+        <v>507</v>
       </c>
       <c r="B50" t="s">
-        <v>115</v>
+        <v>507</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>591</v>
+        <v>626</v>
       </c>
       <c r="D50" t="s">
-        <v>671</v>
+        <v>683</v>
       </c>
       <c r="E50" t="s">
         <v>691</v>
@@ -13677,10 +13677,10 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B51" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>627</v>
@@ -13697,16 +13697,16 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>452</v>
+        <v>478</v>
       </c>
       <c r="B52" t="s">
-        <v>452</v>
+        <v>478</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>628</v>
       </c>
       <c r="D52" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E52" t="s">
         <v>691</v>
@@ -13717,16 +13717,16 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="B53" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>629</v>
       </c>
       <c r="D53" t="s">
-        <v>671</v>
+        <v>684</v>
       </c>
       <c r="E53" t="s">
         <v>691</v>
@@ -13737,10 +13737,10 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>443</v>
+        <v>509</v>
       </c>
       <c r="B54" t="s">
-        <v>443</v>
+        <v>509</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>630</v>
@@ -13757,16 +13757,16 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="B55" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>625</v>
+        <v>631</v>
       </c>
       <c r="D55" t="s">
-        <v>671</v>
+        <v>677</v>
       </c>
       <c r="E55" t="s">
         <v>691</v>
@@ -13777,13 +13777,13 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>441</v>
+        <v>520</v>
       </c>
       <c r="B56" t="s">
-        <v>441</v>
+        <v>520</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="D56" t="s">
         <v>671</v>
@@ -13797,13 +13797,13 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>459</v>
+        <v>445</v>
       </c>
       <c r="B57" t="s">
-        <v>459</v>
+        <v>445</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="D57" t="s">
         <v>671</v>
@@ -13817,16 +13817,16 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>444</v>
+        <v>452</v>
       </c>
       <c r="B58" t="s">
-        <v>444</v>
+        <v>452</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="D58" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="E58" t="s">
         <v>691</v>
@@ -13837,16 +13837,16 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>448</v>
+        <v>487</v>
       </c>
       <c r="B59" t="s">
-        <v>448</v>
+        <v>487</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>634</v>
+        <v>586</v>
       </c>
       <c r="D59" t="s">
-        <v>685</v>
+        <v>671</v>
       </c>
       <c r="E59" t="s">
         <v>691</v>
@@ -13857,16 +13857,16 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>495</v>
+        <v>113</v>
       </c>
       <c r="B60" t="s">
-        <v>495</v>
+        <v>113</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>635</v>
+        <v>588</v>
       </c>
       <c r="D60" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E60" t="s">
         <v>691</v>
@@ -13877,13 +13877,13 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>514</v>
+        <v>112</v>
       </c>
       <c r="B61" t="s">
-        <v>514</v>
+        <v>112</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>636</v>
+        <v>582</v>
       </c>
       <c r="D61" t="s">
         <v>671</v>
@@ -13897,13 +13897,13 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B62" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D62" t="s">
         <v>671</v>
@@ -13917,16 +13917,16 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>496</v>
+        <v>518</v>
       </c>
       <c r="B63" t="s">
-        <v>496</v>
+        <v>518</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D63" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E63" t="s">
         <v>691</v>
@@ -13937,13 +13937,13 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>485</v>
+        <v>459</v>
       </c>
       <c r="B64" t="s">
-        <v>485</v>
+        <v>459</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D64" t="s">
         <v>671</v>
@@ -13957,13 +13957,13 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>467</v>
+        <v>441</v>
       </c>
       <c r="B65" t="s">
-        <v>467</v>
+        <v>441</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="D65" t="s">
         <v>671</v>
@@ -13977,16 +13977,16 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>453</v>
+        <v>502</v>
       </c>
       <c r="B66" t="s">
-        <v>453</v>
+        <v>502</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="D66" t="s">
-        <v>671</v>
+        <v>685</v>
       </c>
       <c r="E66" t="s">
         <v>691</v>
@@ -13997,16 +13997,16 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>471</v>
+        <v>494</v>
       </c>
       <c r="B67" t="s">
-        <v>471</v>
+        <v>494</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="D67" t="s">
-        <v>671</v>
+        <v>686</v>
       </c>
       <c r="E67" t="s">
         <v>691</v>
@@ -14017,16 +14017,16 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>474</v>
+        <v>460</v>
       </c>
       <c r="B68" t="s">
-        <v>474</v>
+        <v>460</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D68" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="E68" t="s">
         <v>691</v>
@@ -14037,16 +14037,16 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>466</v>
+        <v>491</v>
       </c>
       <c r="B69" t="s">
-        <v>466</v>
+        <v>491</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="D69" t="s">
-        <v>687</v>
+        <v>672</v>
       </c>
       <c r="E69" t="s">
         <v>691</v>
@@ -14057,16 +14057,16 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>491</v>
+        <v>511</v>
       </c>
       <c r="B70" t="s">
-        <v>491</v>
+        <v>511</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D70" t="s">
-        <v>672</v>
+        <v>677</v>
       </c>
       <c r="E70" t="s">
         <v>691</v>
@@ -14077,13 +14077,13 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>479</v>
+        <v>454</v>
       </c>
       <c r="B71" t="s">
-        <v>479</v>
+        <v>454</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="D71" t="s">
         <v>671</v>
@@ -14103,7 +14103,7 @@
         <v>481</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="D72" t="s">
         <v>671</v>
@@ -14117,13 +14117,13 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>468</v>
+        <v>493</v>
       </c>
       <c r="B73" t="s">
-        <v>468</v>
+        <v>493</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="D73" t="s">
         <v>671</v>
@@ -14137,16 +14137,16 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>447</v>
+        <v>513</v>
       </c>
       <c r="B74" t="s">
-        <v>447</v>
+        <v>513</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="D74" t="s">
-        <v>688</v>
+        <v>671</v>
       </c>
       <c r="E74" t="s">
         <v>691</v>
@@ -14157,13 +14157,13 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>509</v>
+        <v>465</v>
       </c>
       <c r="B75" t="s">
-        <v>509</v>
+        <v>465</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D75" t="s">
         <v>671</v>
@@ -14177,13 +14177,13 @@
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>518</v>
+        <v>471</v>
       </c>
       <c r="B76" t="s">
-        <v>518</v>
+        <v>471</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="D76" t="s">
         <v>671</v>
@@ -14197,16 +14197,16 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="B77" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="D77" t="s">
-        <v>686</v>
+        <v>671</v>
       </c>
       <c r="E77" t="s">
         <v>691</v>
@@ -14217,13 +14217,13 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>500</v>
+        <v>451</v>
       </c>
       <c r="B78" t="s">
-        <v>500</v>
+        <v>451</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D78" t="s">
         <v>671</v>
@@ -14237,13 +14237,13 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>493</v>
+        <v>470</v>
       </c>
       <c r="B79" t="s">
-        <v>493</v>
+        <v>470</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="D79" t="s">
         <v>671</v>
@@ -14257,16 +14257,16 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>455</v>
+        <v>488</v>
       </c>
       <c r="B80" t="s">
-        <v>455</v>
+        <v>488</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="D80" t="s">
-        <v>671</v>
+        <v>677</v>
       </c>
       <c r="E80" t="s">
         <v>691</v>
@@ -14277,16 +14277,16 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>484</v>
+        <v>466</v>
       </c>
       <c r="B81" t="s">
-        <v>484</v>
+        <v>466</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="D81" t="s">
-        <v>671</v>
+        <v>688</v>
       </c>
       <c r="E81" t="s">
         <v>691</v>
@@ -14297,16 +14297,16 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>456</v>
+        <v>503</v>
       </c>
       <c r="B82" t="s">
-        <v>456</v>
+        <v>503</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="D82" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
       <c r="E82" t="s">
         <v>691</v>
@@ -14317,13 +14317,13 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B83" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="D83" t="s">
         <v>671</v>
@@ -14337,16 +14337,16 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="B84" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D84" t="s">
-        <v>671</v>
+        <v>689</v>
       </c>
       <c r="E84" t="s">
         <v>691</v>
@@ -14357,13 +14357,13 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>505</v>
+        <v>485</v>
       </c>
       <c r="B85" t="s">
-        <v>505</v>
+        <v>485</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="D85" t="s">
         <v>671</v>
@@ -14377,16 +14377,16 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>464</v>
+        <v>495</v>
       </c>
       <c r="B86" t="s">
-        <v>464</v>
+        <v>495</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="D86" t="s">
-        <v>689</v>
+        <v>672</v>
       </c>
       <c r="E86" t="s">
         <v>691</v>
@@ -14397,13 +14397,13 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>519</v>
+        <v>504</v>
       </c>
       <c r="B87" t="s">
-        <v>519</v>
+        <v>504</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="D87" t="s">
         <v>671</v>
@@ -14417,16 +14417,16 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>515</v>
+        <v>456</v>
       </c>
       <c r="B88" t="s">
-        <v>515</v>
+        <v>456</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="D88" t="s">
-        <v>671</v>
+        <v>683</v>
       </c>
       <c r="E88" t="s">
         <v>691</v>
@@ -14437,13 +14437,13 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>458</v>
+        <v>514</v>
       </c>
       <c r="B89" t="s">
-        <v>458</v>
+        <v>514</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="D89" t="s">
         <v>671</v>
@@ -14457,13 +14457,13 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="B90" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="D90" t="s">
         <v>671</v>
@@ -14477,16 +14477,16 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>494</v>
+        <v>443</v>
       </c>
       <c r="B91" t="s">
-        <v>494</v>
+        <v>443</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="D91" t="s">
-        <v>690</v>
+        <v>671</v>
       </c>
       <c r="E91" t="s">
         <v>691</v>
@@ -14497,13 +14497,13 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B92" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="D92" t="s">
         <v>671</v>
@@ -14517,13 +14517,13 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>120</v>
+        <v>500</v>
       </c>
       <c r="B93" t="s">
-        <v>120</v>
+        <v>500</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>586</v>
+        <v>666</v>
       </c>
       <c r="D93" t="s">
         <v>671</v>
@@ -14537,13 +14537,13 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>112</v>
+        <v>516</v>
       </c>
       <c r="B94" t="s">
-        <v>112</v>
+        <v>516</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>588</v>
+        <v>667</v>
       </c>
       <c r="D94" t="s">
         <v>671</v>
@@ -14557,16 +14557,16 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>498</v>
+        <v>447</v>
       </c>
       <c r="B95" t="s">
-        <v>498</v>
+        <v>447</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>668</v>
       </c>
       <c r="D95" t="s">
-        <v>671</v>
+        <v>690</v>
       </c>
       <c r="E95" t="s">
         <v>691</v>
@@ -14577,10 +14577,10 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>489</v>
+        <v>458</v>
       </c>
       <c r="B96" t="s">
-        <v>489</v>
+        <v>458</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>669</v>
@@ -14597,16 +14597,16 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>516</v>
+        <v>462</v>
       </c>
       <c r="B97" t="s">
-        <v>516</v>
+        <v>462</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>670</v>
       </c>
       <c r="D97" t="s">
-        <v>671</v>
+        <v>681</v>
       </c>
       <c r="E97" t="s">
         <v>691</v>
@@ -14649,7 +14649,7 @@
     <hyperlink ref="F16" r:id="rId30" location="isAssociatedWith"/>
     <hyperlink ref="C17" r:id="rId31"/>
     <hyperlink ref="F17" r:id="rId32" location="isAssociatedWith"/>
-    <hyperlink ref="C18" r:id="rId33" location="doi"/>
+    <hyperlink ref="C18" r:id="rId33"/>
     <hyperlink ref="F18" r:id="rId34" location="isAssociatedWith"/>
     <hyperlink ref="C19" r:id="rId35"/>
     <hyperlink ref="F19" r:id="rId36" location="isAssociatedWith"/>
@@ -14713,7 +14713,7 @@
     <hyperlink ref="F48" r:id="rId94" location="isAssociatedWith"/>
     <hyperlink ref="C49" r:id="rId95"/>
     <hyperlink ref="F49" r:id="rId96" location="isAssociatedWith"/>
-    <hyperlink ref="C50" r:id="rId97"/>
+    <hyperlink ref="C50" r:id="rId97" location="doi"/>
     <hyperlink ref="F50" r:id="rId98" location="isAssociatedWith"/>
     <hyperlink ref="C51" r:id="rId99"/>
     <hyperlink ref="F51" r:id="rId100" location="isAssociatedWith"/>
@@ -14777,7 +14777,7 @@
     <hyperlink ref="F80" r:id="rId158" location="isAssociatedWith"/>
     <hyperlink ref="C81" r:id="rId159"/>
     <hyperlink ref="F81" r:id="rId160" location="isAssociatedWith"/>
-    <hyperlink ref="C82" r:id="rId161" location="wasUpdatedBy"/>
+    <hyperlink ref="C82" r:id="rId161"/>
     <hyperlink ref="F82" r:id="rId162" location="isAssociatedWith"/>
     <hyperlink ref="C83" r:id="rId163"/>
     <hyperlink ref="F83" r:id="rId164" location="isAssociatedWith"/>
@@ -14789,7 +14789,7 @@
     <hyperlink ref="F86" r:id="rId170" location="isAssociatedWith"/>
     <hyperlink ref="C87" r:id="rId171"/>
     <hyperlink ref="F87" r:id="rId172" location="isAssociatedWith"/>
-    <hyperlink ref="C88" r:id="rId173"/>
+    <hyperlink ref="C88" r:id="rId173" location="wasUpdatedBy"/>
     <hyperlink ref="F88" r:id="rId174" location="isAssociatedWith"/>
     <hyperlink ref="C89" r:id="rId175"/>
     <hyperlink ref="F89" r:id="rId176" location="isAssociatedWith"/>

</xml_diff>